<commit_message>
Atualização do arquivo considerando os coordenadores de compra como alçada 3
</commit_message>
<xml_diff>
--- a/filiais.xlsx
+++ b/filiais.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pucpredu-my.sharepoint.com/personal/ramon_roldan_grupomarista_org_br/Documents/Desktop/Alcadas_dos_Compradores_Temporarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="13_ncr:1_{AA18D564-878F-465F-AF4D-D75B1A918F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{EE237FBA-E4F8-4AFF-8C99-9852C4575135}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{AA18D564-878F-465F-AF4D-D75B1A918F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE1A93A2-506A-40F5-A3F9-57A9AADDA48A}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="490" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="490" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="usuarios" sheetId="3" r:id="rId1"/>
@@ -553,8 +553,15 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -620,7 +627,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -636,6 +643,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1022,7 +1032,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37674D7C-A3F8-4AA2-A1B8-D6A04DC6DE4A}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
@@ -2860,7 +2870,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3149,7 +3161,7 @@
         <v>161</v>
       </c>
       <c r="B26" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>167</v>
@@ -3160,7 +3172,7 @@
         <v>162</v>
       </c>
       <c r="B27" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>167</v>
@@ -3171,7 +3183,7 @@
         <v>163</v>
       </c>
       <c r="B28" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>167</v>
@@ -3314,7 +3326,7 @@
         <v>161</v>
       </c>
       <c r="B41" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C41" s="5" t="s">
         <v>168</v>
@@ -3325,7 +3337,7 @@
         <v>162</v>
       </c>
       <c r="B42" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C42" s="5" t="s">
         <v>168</v>
@@ -3336,7 +3348,7 @@
         <v>163</v>
       </c>
       <c r="B43" s="5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>168</v>
@@ -3347,7 +3359,7 @@
         <v>164</v>
       </c>
       <c r="B44" s="5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C44" s="5" t="s">
         <v>168</v>
@@ -3490,7 +3502,7 @@
         <v>161</v>
       </c>
       <c r="B57" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C57" s="6" t="s">
         <v>169</v>
@@ -3501,7 +3513,7 @@
         <v>162</v>
       </c>
       <c r="B58" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C58" s="6" t="s">
         <v>169</v>
@@ -3512,7 +3524,7 @@
         <v>163</v>
       </c>
       <c r="B59" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C59" s="6" t="s">
         <v>169</v>
@@ -3522,8 +3534,8 @@
       <c r="A60" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="B60" s="6">
-        <v>3</v>
+      <c r="B60" s="7">
+        <v>4</v>
       </c>
       <c r="C60" s="6" t="s">
         <v>169</v>
@@ -3534,7 +3546,7 @@
         <v>165</v>
       </c>
       <c r="B61" s="6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C61" s="6" t="s">
         <v>169</v>
@@ -3542,7 +3554,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
rodando atualizacao, devido a mudança no quadro de funcionarios da SOS.
</commit_message>
<xml_diff>
--- a/filiais.xlsx
+++ b/filiais.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pucpredu-my.sharepoint.com/personal/ramon_roldan_grupomarista_org_br/Documents/Desktop/Alcadas_dos_Compradores_Temporarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="17" documentId="13_ncr:1_{AA18D564-878F-465F-AF4D-D75B1A918F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FE1A93A2-506A-40F5-A3F9-57A9AADDA48A}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="13_ncr:1_{AA18D564-878F-465F-AF4D-D75B1A918F62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4C1204D1-8A7E-492E-8ED7-272A07F125F2}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="490" windowWidth="19420" windowHeight="10420" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="171">
   <si>
     <t>HANDLE</t>
   </si>
@@ -547,6 +547,9 @@
   </si>
   <si>
     <t>OC -SOS TELECOM – SUPRIMENTOS 4 ACIMA DE R$ 2.000.000,01</t>
+  </si>
+  <si>
+    <t>pires.alessandra</t>
   </si>
 </sst>
 </file>
@@ -600,7 +603,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -623,11 +626,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -645,7 +663,22 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2870,685 +2903,686 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63"/>
+    <sheetView tabSelected="1" zoomScale="53" zoomScaleNormal="53" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.54296875" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="63.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="19.26953125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.08984375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="11.54296875" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="7" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="8" t="s">
         <v>149</v>
       </c>
-      <c r="B2" s="3">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="B2" s="8">
+        <v>1</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="8" t="s">
         <v>150</v>
       </c>
-      <c r="B3" s="3">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="B3" s="8">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B4" s="3">
-        <v>1</v>
-      </c>
-      <c r="C4" s="3" t="s">
+      <c r="A4" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B4" s="8">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="B5" s="3">
-        <v>1</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="B5" s="8">
+        <v>1</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="B6" s="3">
-        <v>1</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="B6" s="8">
+        <v>1</v>
+      </c>
+      <c r="C6" s="8" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+      <c r="A7" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="B7" s="3">
-        <v>1</v>
-      </c>
-      <c r="C7" s="3" t="s">
+      <c r="B7" s="8">
+        <v>1</v>
+      </c>
+      <c r="C7" s="8" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="B8" s="3">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="B8" s="8">
+        <v>1</v>
+      </c>
+      <c r="C8" s="8" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+      <c r="A9" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="B9" s="3">
-        <v>1</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="B9" s="8">
+        <v>1</v>
+      </c>
+      <c r="C9" s="8" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
+      <c r="A10" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="B10" s="3">
-        <v>1</v>
-      </c>
-      <c r="C10" s="3" t="s">
+      <c r="B10" s="8">
+        <v>1</v>
+      </c>
+      <c r="C10" s="8" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="B11" s="3">
-        <v>1</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="B11" s="8">
+        <v>1</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="B12" s="3">
-        <v>2</v>
-      </c>
-      <c r="C12" s="3" t="s">
+      <c r="B12" s="8">
+        <v>2</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="3" t="s">
+      <c r="A13" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="B13" s="3">
-        <v>2</v>
-      </c>
-      <c r="C13" s="3" t="s">
+      <c r="B13" s="8">
+        <v>2</v>
+      </c>
+      <c r="C13" s="8" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="B14" s="4">
-        <v>1</v>
-      </c>
-      <c r="C14" s="4" t="s">
+      <c r="B14" s="9">
+        <v>1</v>
+      </c>
+      <c r="C14" s="9" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="B15" s="4">
-        <v>1</v>
-      </c>
-      <c r="C15" s="4" t="s">
+      <c r="B15" s="9">
+        <v>1</v>
+      </c>
+      <c r="C15" s="9" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="B16" s="4">
-        <v>1</v>
-      </c>
-      <c r="C16" s="4" t="s">
+      <c r="A16" s="9" t="s">
+        <v>170</v>
+      </c>
+      <c r="B16" s="9">
+        <v>1</v>
+      </c>
+      <c r="C16" s="9" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="B17" s="4">
-        <v>1</v>
-      </c>
-      <c r="C17" s="4" t="s">
+      <c r="B17" s="9">
+        <v>1</v>
+      </c>
+      <c r="C17" s="9" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+      <c r="A18" s="9" t="s">
         <v>153</v>
       </c>
-      <c r="B18" s="4">
-        <v>1</v>
-      </c>
-      <c r="C18" s="4" t="s">
+      <c r="B18" s="9">
+        <v>1</v>
+      </c>
+      <c r="C18" s="9" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="A19" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="B19" s="4">
-        <v>1</v>
-      </c>
-      <c r="C19" s="4" t="s">
+      <c r="B19" s="9">
+        <v>1</v>
+      </c>
+      <c r="C19" s="9" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="B20" s="4">
-        <v>1</v>
-      </c>
-      <c r="C20" s="4" t="s">
+      <c r="B20" s="9">
+        <v>1</v>
+      </c>
+      <c r="C20" s="9" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="4" t="s">
+      <c r="A21" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="B21" s="4">
-        <v>1</v>
-      </c>
-      <c r="C21" s="4" t="s">
+      <c r="B21" s="9">
+        <v>1</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="9" t="s">
         <v>157</v>
       </c>
-      <c r="B22" s="4">
-        <v>1</v>
-      </c>
-      <c r="C22" s="4" t="s">
+      <c r="B22" s="9">
+        <v>1</v>
+      </c>
+      <c r="C22" s="9" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="4" t="s">
+      <c r="A23" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B23" s="4">
-        <v>1</v>
-      </c>
-      <c r="C23" s="4" t="s">
+      <c r="B23" s="9">
+        <v>1</v>
+      </c>
+      <c r="C23" s="9" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="9" t="s">
         <v>159</v>
       </c>
-      <c r="B24" s="4">
-        <v>2</v>
-      </c>
-      <c r="C24" s="4" t="s">
+      <c r="B24" s="9">
+        <v>2</v>
+      </c>
+      <c r="C24" s="9" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="B25" s="4">
-        <v>2</v>
-      </c>
-      <c r="C25" s="4" t="s">
+      <c r="B25" s="9">
+        <v>2</v>
+      </c>
+      <c r="C25" s="9" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="9" t="s">
         <v>161</v>
       </c>
-      <c r="B26" s="4">
-        <v>3</v>
-      </c>
-      <c r="C26" s="4" t="s">
+      <c r="B26" s="9">
+        <v>3</v>
+      </c>
+      <c r="C26" s="9" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="A27" s="9" t="s">
         <v>162</v>
       </c>
-      <c r="B27" s="4">
-        <v>3</v>
-      </c>
-      <c r="C27" s="4" t="s">
+      <c r="B27" s="9">
+        <v>3</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="A28" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="B28" s="4">
-        <v>3</v>
-      </c>
-      <c r="C28" s="4" t="s">
+      <c r="B28" s="9">
+        <v>3</v>
+      </c>
+      <c r="C28" s="9" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="B29" s="5">
-        <v>1</v>
-      </c>
-      <c r="C29" s="5" t="s">
+      <c r="B29" s="10">
+        <v>1</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
+      <c r="A30" s="10" t="s">
         <v>150</v>
       </c>
-      <c r="B30" s="5">
-        <v>1</v>
-      </c>
-      <c r="C30" s="5" t="s">
+      <c r="B30" s="10">
+        <v>1</v>
+      </c>
+      <c r="C30" s="10" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>151</v>
-      </c>
-      <c r="B31" s="5">
-        <v>1</v>
-      </c>
-      <c r="C31" s="5" t="s">
+      <c r="A31" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="B31" s="10">
+        <v>1</v>
+      </c>
+      <c r="C31" s="10" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
+      <c r="A32" s="10" t="s">
         <v>152</v>
       </c>
-      <c r="B32" s="5">
-        <v>1</v>
-      </c>
-      <c r="C32" s="5" t="s">
+      <c r="B32" s="10">
+        <v>1</v>
+      </c>
+      <c r="C32" s="10" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="10" t="s">
         <v>153</v>
       </c>
-      <c r="B33" s="5">
-        <v>1</v>
-      </c>
-      <c r="C33" s="5" t="s">
+      <c r="B33" s="10">
+        <v>1</v>
+      </c>
+      <c r="C33" s="10" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="B34" s="5">
-        <v>1</v>
-      </c>
-      <c r="C34" s="5" t="s">
+      <c r="B34" s="10">
+        <v>1</v>
+      </c>
+      <c r="C34" s="10" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
+      <c r="A35" s="10" t="s">
         <v>155</v>
       </c>
-      <c r="B35" s="5">
-        <v>1</v>
-      </c>
-      <c r="C35" s="5" t="s">
+      <c r="B35" s="10">
+        <v>1</v>
+      </c>
+      <c r="C35" s="10" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
+      <c r="A36" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="B36" s="5">
-        <v>1</v>
-      </c>
-      <c r="C36" s="5" t="s">
+      <c r="B36" s="10">
+        <v>1</v>
+      </c>
+      <c r="C36" s="10" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="5" t="s">
+      <c r="A37" s="10" t="s">
         <v>157</v>
       </c>
-      <c r="B37" s="5">
-        <v>1</v>
-      </c>
-      <c r="C37" s="5" t="s">
+      <c r="B37" s="10">
+        <v>1</v>
+      </c>
+      <c r="C37" s="10" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+      <c r="A38" s="10" t="s">
         <v>158</v>
       </c>
-      <c r="B38" s="5">
-        <v>1</v>
-      </c>
-      <c r="C38" s="5" t="s">
+      <c r="B38" s="10">
+        <v>1</v>
+      </c>
+      <c r="C38" s="10" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+      <c r="A39" s="10" t="s">
         <v>159</v>
       </c>
-      <c r="B39" s="5">
-        <v>2</v>
-      </c>
-      <c r="C39" s="5" t="s">
+      <c r="B39" s="10">
+        <v>2</v>
+      </c>
+      <c r="C39" s="10" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
+      <c r="A40" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="B40" s="5">
-        <v>2</v>
-      </c>
-      <c r="C40" s="5" t="s">
+      <c r="B40" s="10">
+        <v>2</v>
+      </c>
+      <c r="C40" s="10" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+      <c r="A41" s="10" t="s">
         <v>161</v>
       </c>
-      <c r="B41" s="5">
-        <v>3</v>
-      </c>
-      <c r="C41" s="5" t="s">
+      <c r="B41" s="10">
+        <v>3</v>
+      </c>
+      <c r="C41" s="10" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
+      <c r="A42" s="10" t="s">
         <v>162</v>
       </c>
-      <c r="B42" s="5">
-        <v>3</v>
-      </c>
-      <c r="C42" s="5" t="s">
+      <c r="B42" s="10">
+        <v>3</v>
+      </c>
+      <c r="C42" s="10" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
+      <c r="A43" s="10" t="s">
         <v>163</v>
       </c>
-      <c r="B43" s="5">
-        <v>3</v>
-      </c>
-      <c r="C43" s="5" t="s">
+      <c r="B43" s="10">
+        <v>3</v>
+      </c>
+      <c r="C43" s="10" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="5" t="s">
+      <c r="A44" s="10" t="s">
         <v>164</v>
       </c>
-      <c r="B44" s="5">
+      <c r="B44" s="10">
         <v>4</v>
       </c>
-      <c r="C44" s="5" t="s">
+      <c r="C44" s="10" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="6" t="s">
+      <c r="A45" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="B45" s="6">
-        <v>1</v>
-      </c>
-      <c r="C45" s="6" t="s">
+      <c r="B45" s="11">
+        <v>1</v>
+      </c>
+      <c r="C45" s="11" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
+      <c r="A46" s="11" t="s">
         <v>150</v>
       </c>
-      <c r="B46" s="6">
-        <v>1</v>
-      </c>
-      <c r="C46" s="6" t="s">
+      <c r="B46" s="11">
+        <v>1</v>
+      </c>
+      <c r="C46" s="11" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="B47" s="6">
-        <v>1</v>
-      </c>
-      <c r="C47" s="6" t="s">
+      <c r="A47" s="11" t="s">
+        <v>170</v>
+      </c>
+      <c r="B47" s="11">
+        <v>1</v>
+      </c>
+      <c r="C47" s="11" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="6" t="s">
+      <c r="A48" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="B48" s="6">
-        <v>1</v>
-      </c>
-      <c r="C48" s="6" t="s">
+      <c r="B48" s="11">
+        <v>1</v>
+      </c>
+      <c r="C48" s="11" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="B49" s="6">
-        <v>1</v>
-      </c>
-      <c r="C49" s="6" t="s">
+      <c r="B49" s="11">
+        <v>1</v>
+      </c>
+      <c r="C49" s="11" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
+      <c r="A50" s="11" t="s">
         <v>154</v>
       </c>
-      <c r="B50" s="6">
-        <v>1</v>
-      </c>
-      <c r="C50" s="6" t="s">
+      <c r="B50" s="11">
+        <v>1</v>
+      </c>
+      <c r="C50" s="11" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="6" t="s">
+      <c r="A51" s="11" t="s">
         <v>155</v>
       </c>
-      <c r="B51" s="6">
-        <v>1</v>
-      </c>
-      <c r="C51" s="6" t="s">
+      <c r="B51" s="11">
+        <v>1</v>
+      </c>
+      <c r="C51" s="11" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="6" t="s">
+      <c r="A52" s="11" t="s">
         <v>156</v>
       </c>
-      <c r="B52" s="6">
-        <v>1</v>
-      </c>
-      <c r="C52" s="6" t="s">
+      <c r="B52" s="11">
+        <v>1</v>
+      </c>
+      <c r="C52" s="11" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="6" t="s">
+      <c r="A53" s="11" t="s">
         <v>157</v>
       </c>
-      <c r="B53" s="6">
-        <v>1</v>
-      </c>
-      <c r="C53" s="6" t="s">
+      <c r="B53" s="11">
+        <v>1</v>
+      </c>
+      <c r="C53" s="11" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="6" t="s">
+      <c r="A54" s="11" t="s">
         <v>158</v>
       </c>
-      <c r="B54" s="6">
-        <v>1</v>
-      </c>
-      <c r="C54" s="6" t="s">
+      <c r="B54" s="11">
+        <v>1</v>
+      </c>
+      <c r="C54" s="11" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="6" t="s">
+      <c r="A55" s="11" t="s">
         <v>159</v>
       </c>
-      <c r="B55" s="6">
-        <v>2</v>
-      </c>
-      <c r="C55" s="6" t="s">
+      <c r="B55" s="11">
+        <v>2</v>
+      </c>
+      <c r="C55" s="11" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="6" t="s">
+      <c r="A56" s="11" t="s">
         <v>160</v>
       </c>
-      <c r="B56" s="6">
-        <v>2</v>
-      </c>
-      <c r="C56" s="6" t="s">
+      <c r="B56" s="11">
+        <v>2</v>
+      </c>
+      <c r="C56" s="11" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="6" t="s">
+      <c r="A57" s="11" t="s">
         <v>161</v>
       </c>
-      <c r="B57" s="6">
-        <v>3</v>
-      </c>
-      <c r="C57" s="6" t="s">
+      <c r="B57" s="11">
+        <v>3</v>
+      </c>
+      <c r="C57" s="11" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="6" t="s">
+      <c r="A58" s="11" t="s">
         <v>162</v>
       </c>
-      <c r="B58" s="6">
-        <v>3</v>
-      </c>
-      <c r="C58" s="6" t="s">
+      <c r="B58" s="11">
+        <v>3</v>
+      </c>
+      <c r="C58" s="11" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="6" t="s">
+      <c r="A59" s="11" t="s">
         <v>163</v>
       </c>
-      <c r="B59" s="6">
-        <v>3</v>
-      </c>
-      <c r="C59" s="6" t="s">
+      <c r="B59" s="11">
+        <v>3</v>
+      </c>
+      <c r="C59" s="11" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="6" t="s">
+      <c r="A60" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="B60" s="7">
+      <c r="B60" s="12">
         <v>4</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C60" s="11" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="6" t="s">
+      <c r="A61" s="11" t="s">
         <v>165</v>
       </c>
-      <c r="B61" s="6">
+      <c r="B61" s="11">
         <v>5</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C61" s="11" t="s">
         <v>169</v>
       </c>
     </row>

</xml_diff>